<commit_message>
Attack Of The Websockets Part II - Revenge Of The RMI
</commit_message>
<xml_diff>
--- a/sd_checklist_meta2.xlsx
+++ b/sd_checklist_meta2.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raul/Home/Git2018/SDIST/projeto_meta_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bloodeon\Documents\Projects\projectRMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="460" windowWidth="28820" windowHeight="21140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016-2017" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>REST</t>
   </si>
@@ -168,13 +168,16 @@
   </si>
   <si>
     <t>Associar conta existente ao Facebook</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -383,6 +386,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -694,7 +700,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -738,7 +744,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -759,28 +765,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="75.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:70" s="5" customFormat="1">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -788,7 +794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:70" s="5" customFormat="1">
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -796,7 +802,7 @@
         <v>2017987654</v>
       </c>
     </row>
-    <row r="5" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:70" s="5" customFormat="1">
       <c r="A5" s="5">
         <f>A6+A21+A25+A31</f>
         <v>100</v>
@@ -810,7 +816,7 @@
       </c>
       <c r="D5" s="5">
         <f t="shared" ref="D5:BO5" si="0">D6+D21+D25+D31+D37+D42</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
@@ -1077,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="A6" s="1">
         <f>SUM(A7:A20)</f>
         <v>55</v>
@@ -1091,7 +1097,7 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" ref="D6:BO6" si="2">SUM(D7:D20)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="2"/>
@@ -1358,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1368,8 +1374,11 @@
       <c r="C7" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -1379,8 +1388,11 @@
       <c r="C8" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -1390,8 +1402,11 @@
       <c r="C9" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A10" s="3">
         <v>5</v>
       </c>
@@ -1401,8 +1416,11 @@
       <c r="C10" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -1412,8 +1430,11 @@
       <c r="C11" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A12" s="3">
         <v>5</v>
       </c>
@@ -1423,8 +1444,11 @@
       <c r="C12" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A13" s="3">
         <v>5</v>
       </c>
@@ -1434,8 +1458,11 @@
       <c r="C13" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D13" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A14" s="3">
         <v>5</v>
       </c>
@@ -1445,8 +1472,11 @@
       <c r="C14" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A15" s="3">
         <v>5</v>
       </c>
@@ -1456,8 +1486,11 @@
       <c r="C15" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D15" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A16" s="3">
         <v>5</v>
       </c>
@@ -1467,8 +1500,11 @@
       <c r="C16" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D16" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A17" s="3">
         <v>5</v>
       </c>
@@ -1478,8 +1514,11 @@
       <c r="C17" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D17" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A18" s="3">
         <v>0</v>
       </c>
@@ -1490,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A19" s="3">
         <v>0</v>
       </c>
@@ -1501,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A20" s="3">
         <v>0</v>
       </c>
@@ -1512,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="A21" s="1">
         <f>SUM(A22:A24)</f>
         <v>15</v>
@@ -1526,7 +1565,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" ref="D21:BO21" si="4">SUM(D22:D24)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="4"/>
@@ -1793,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A22" s="3">
         <v>5</v>
       </c>
@@ -1804,7 +1843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A23" s="3">
         <v>5</v>
       </c>
@@ -1815,7 +1854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A24" s="3">
         <v>5</v>
       </c>
@@ -1825,8 +1864,11 @@
       <c r="C24" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D24" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="A25" s="1">
         <f>SUM(A26:A30)</f>
         <v>20</v>
@@ -1840,7 +1882,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="6"/>
@@ -2107,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A26" s="3">
         <v>5</v>
       </c>
@@ -2117,8 +2159,11 @@
       <c r="C26" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D26" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A27" s="3">
         <v>5</v>
       </c>
@@ -2128,8 +2173,11 @@
       <c r="C27" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D27" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A28" s="3">
         <v>5</v>
       </c>
@@ -2139,8 +2187,11 @@
       <c r="C28" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A29" s="3">
         <v>5</v>
       </c>
@@ -2151,7 +2202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A30" s="3">
         <v>0</v>
       </c>
@@ -2162,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="A31" s="1">
         <f>SUM(A32:A36)</f>
         <v>10</v>
@@ -2176,7 +2227,7 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" ref="D31:BO31" si="8">SUM(D32:D36)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="8"/>
@@ -2443,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -2453,8 +2504,11 @@
       <c r="C32" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D32" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -2464,8 +2518,11 @@
       <c r="C33" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D33" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A34" s="3">
         <v>2</v>
       </c>
@@ -2475,8 +2532,11 @@
       <c r="C34" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D34" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A35" s="3">
         <v>2</v>
       </c>
@@ -2486,8 +2546,11 @@
       <c r="C35" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D35" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="A36" s="3">
         <v>2</v>
       </c>
@@ -2497,8 +2560,11 @@
       <c r="C36" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D36" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="B37" s="2" t="s">
         <v>10</v>
       </c>
@@ -2775,23 +2841,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B38" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B39" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:70" s="3" customFormat="1" ht="18.75"/>
+    <row r="41" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B41" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="B42" s="2" t="s">
         <v>12</v>
       </c>
@@ -3068,32 +3134,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B43" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B44" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B45" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B46" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B47" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="B48" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>